<commit_message>
Comments Sun Templates WorkManager in MainActivity
</commit_message>
<xml_diff>
--- a/KOTLIN/_Doc_Kotlin/Kotlin_School.xlsx
+++ b/KOTLIN/_Doc_Kotlin/Kotlin_School.xlsx
@@ -3,26 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB24B7F7-ACB2-46B3-B89B-CE1CA927AB6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C69473-9E43-455B-8CBB-1C2721C176BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="844" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LINKS INFO" sheetId="1" r:id="rId1"/>
-    <sheet name="Kotlin Bootcamp" sheetId="2" r:id="rId2"/>
-    <sheet name="DOCUMENTATION" sheetId="3" r:id="rId3"/>
-    <sheet name="Kotlin in Action" sheetId="4" r:id="rId4"/>
-    <sheet name="The Joy of Kotlin" sheetId="5" r:id="rId5"/>
-    <sheet name="Kotlin Ботаник Джон Скин" sheetId="6" r:id="rId6"/>
-    <sheet name="Head First Kotlin" sheetId="7" r:id="rId7"/>
-    <sheet name="DevColibry" sheetId="8" r:id="rId8"/>
-    <sheet name="Дударь" sheetId="9" r:id="rId9"/>
-    <sheet name="ЗАДАЧКИ" sheetId="10" r:id="rId10"/>
+    <sheet name="Лист1" sheetId="11" r:id="rId1"/>
+    <sheet name="LINKS INFO" sheetId="1" r:id="rId2"/>
+    <sheet name="Kotlin Bootcamp" sheetId="2" r:id="rId3"/>
+    <sheet name="DOCUMENTATION" sheetId="3" r:id="rId4"/>
+    <sheet name="Kotlin in Action" sheetId="4" r:id="rId5"/>
+    <sheet name="The Joy of Kotlin" sheetId="5" r:id="rId6"/>
+    <sheet name="Kotlin Ботаник Джон Скин" sheetId="6" r:id="rId7"/>
+    <sheet name="Head First Kotlin" sheetId="7" r:id="rId8"/>
+    <sheet name="DevColibry" sheetId="8" r:id="rId9"/>
+    <sheet name="Дударь" sheetId="9" r:id="rId10"/>
+    <sheet name="ЗАДАЧКИ" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="reviews_ge_anchor" localSheetId="6">'Head First Kotlin'!$C$14</definedName>
-    <definedName name="selected_pages_anchor" localSheetId="6">'Head First Kotlin'!$C$23</definedName>
-    <definedName name="toc_anchor" localSheetId="6">'Head First Kotlin'!$C$46</definedName>
+    <definedName name="reviews_ge_anchor" localSheetId="7">'Head First Kotlin'!$C$14</definedName>
+    <definedName name="selected_pages_anchor" localSheetId="7">'Head First Kotlin'!$C$23</definedName>
+    <definedName name="toc_anchor" localSheetId="7">'Head First Kotlin'!$C$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="3716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="3803">
   <si>
     <t>09.01.2019 - 19.01.2019 -</t>
   </si>
@@ -11274,12 +11275,273 @@
   <si>
     <t>Connect with the data</t>
   </si>
+  <si>
+    <t>Источник</t>
+  </si>
+  <si>
+    <t>TEMPLATES AS 4/1/1</t>
+  </si>
+  <si>
+    <t>Theme.MaterialComponents.DayNight.DarkActionBar</t>
+  </si>
+  <si>
+    <t>No Activity</t>
+  </si>
+  <si>
+    <t>com.google.android.material:material:1.1.1</t>
+  </si>
+  <si>
+    <t>Bacic Activity</t>
+  </si>
+  <si>
+    <t>Material, ConstraintLyout,Navigation-fragment+ui</t>
+  </si>
+  <si>
+    <t>Navigation = 2 экрана с класс переходами SupportActionBar FAB menu три точки SnackBar</t>
+  </si>
+  <si>
+    <t>Botton_Navigation_Activity</t>
+  </si>
+  <si>
+    <t>Два фрагмента и переход между ними по button через NavHostFragment в include + menu… + fab</t>
+  </si>
+  <si>
+    <t>Navigation = 3 экрана без переходов setupActionBarWithNavController FAB menu три точки SnackBar ВСЕ с VIEWMODEL  homeViewModel.text.observe : LiveData&lt;String&gt;</t>
+  </si>
+  <si>
+    <t>Material, ConstraintLyout,Navigation-fragment+ui Lificycle - livedata+viewmodel,</t>
+  </si>
+  <si>
+    <t>Без модулей</t>
+  </si>
+  <si>
+    <t>Примечание</t>
+  </si>
+  <si>
+    <t>Компоновка</t>
+  </si>
+  <si>
+    <t>По 3-м каталогам Fragment+ViewModel и MainActivity в корне</t>
+  </si>
+  <si>
+    <t>Compose_Activity_Preview</t>
+  </si>
+  <si>
+    <t>Material, androidx.ui:ui-layout + material + tooling 0.1.0-dev13</t>
+  </si>
+  <si>
+    <t>Без Lyout рисует прямо из Котлина</t>
+  </si>
+  <si>
+    <t>Theme, Color, Shape, Type пишутся в Котлине</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kotlin 1.3.72 c Warning </t>
+  </si>
+  <si>
+    <t>Hello ANDROID??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material.bottomnavigation.BottomNavigationView Меню перключения  трех фагментов внизу + переход туда же через три точки Слайдера НЕТ </t>
+  </si>
+  <si>
+    <t>Повторно-ошибочные 2 implementation Не изображается menu… - забыли включить</t>
+  </si>
+  <si>
+    <t>Fullscreen_Activity</t>
+  </si>
+  <si>
+    <t>11 шт deprecated</t>
+  </si>
+  <si>
+    <t>Material, Frame+LinearLyout</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Устройство</t>
+  </si>
+  <si>
+    <t>Тема</t>
+  </si>
+  <si>
+    <t>implementation</t>
+  </si>
+  <si>
+    <t>Activity+XML</t>
+  </si>
+  <si>
+    <t>При нажатии на экран полностью его переводи в FULL ; стрелка &lt;--</t>
+  </si>
+  <si>
+    <t>Google_AdMob_Ads_Activity</t>
+  </si>
+  <si>
+    <t>Не стартует - нет манифеста и json</t>
+  </si>
+  <si>
+    <t>Material, play-services-ads+ RelativeLayout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* https://googlemobileadssdk.page.link/admob-android-update-manifest </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://googlemobileadssdk.page.link/ad-manager-android-update-manifest</t>
+  </si>
+  <si>
+    <t>Google_Maps_Activity</t>
+  </si>
+  <si>
+    <t>Material, play-services-maps+constraintlayout</t>
+  </si>
+  <si>
+    <t>Стартует пустой экран need a Google Maps API key</t>
+  </si>
+  <si>
+    <t>Material, ConstraintLyout,  Lificycle - livedata+viewmodel, annotanion</t>
+  </si>
+  <si>
+    <t>Data( Model+ repo…) + Ui.login 7 файловd в т.ч Model+factory + XML</t>
+  </si>
+  <si>
+    <t>Берет Email+Pass и Все - в сле раз проверяет наверное</t>
+  </si>
+  <si>
+    <t>Login_Activity</t>
+  </si>
+  <si>
+    <t>Data( Model+ repo…) + Ui.login 7 файловd в т.ч LoginViewModel+factory + XML + observe + ProgressBar Мощная обработка диалога</t>
+  </si>
+  <si>
+    <t>Master-Detail_Flow</t>
+  </si>
+  <si>
+    <t>Material,Recycler,appcompat</t>
+  </si>
+  <si>
+    <t>NestedScrollView, coordinatorlayout,  CollapsingToolbarLayout, FloatingActionButton, RecyclerView</t>
+  </si>
+  <si>
+    <t>Три котлин Большие + Объект DummyContent;  Три XML + 3 item_list.XML</t>
+  </si>
+  <si>
+    <t>Перечень деталей с раскрытием описания детали</t>
+  </si>
+  <si>
+    <t>Годится без JetPack Класс recyclerview и Bundle</t>
+  </si>
+  <si>
+    <t>Navigation_Drawer_Activity</t>
+  </si>
+  <si>
+    <t>Бутерброд который переключает три фрагмента в navigation</t>
+  </si>
+  <si>
+    <t>Navigation с 3 фрагментами без переходов; Main в корне + XML c include и material.navigation.NavigationView + MutableLiveData+ observe</t>
+  </si>
+  <si>
+    <t>Setting_Activity</t>
+  </si>
+  <si>
+    <t>preference:preference нужно ktx</t>
+  </si>
+  <si>
+    <t>Material,preference:preference</t>
+  </si>
+  <si>
+    <t>Main+XML+XML(preference)</t>
+  </si>
+  <si>
+    <t>Спец класс-фрагмент preference со своим xml - спец</t>
+  </si>
+  <si>
+    <t>Что делает неясно - что-тос email - разбирать</t>
+  </si>
+  <si>
+    <t>Scrolling_Activity</t>
+  </si>
+  <si>
+    <t>Material,appcompat</t>
+  </si>
+  <si>
+    <t>NestedScrollView</t>
+  </si>
+  <si>
+    <t>Скролл текст и скрывающийся забавно АФИ с уменьшающимся заголовок</t>
+  </si>
+  <si>
+    <t>Activity+XML с инклюде</t>
+  </si>
+  <si>
+    <t>Tabbed_Activity</t>
+  </si>
+  <si>
+    <t>Material, ConstraintLyout Lificycle - livedata+viewmodel,</t>
+  </si>
+  <si>
+    <t>material.tabs.TabLayout + widget.ViewPager через адаптер из kotlin</t>
+  </si>
+  <si>
+    <t>д.б viewpager 2 весна 2019 @Deprecated FragmentPagerAdapter</t>
+  </si>
+  <si>
+    <t>СЛАЙДЕР на старом viewPager без заголовка и неясно откуда берутся фрагменты</t>
+  </si>
+  <si>
+    <t>Main+UI=(Fragment-ViewModel-Adapter) + 2 XML</t>
+  </si>
+  <si>
+    <t>Fragment+ViewModel</t>
+  </si>
+  <si>
+    <t>Заготовка Фрагмент +  viewModel</t>
+  </si>
+  <si>
+    <t>Засвечивает XML Main и затем заменяет его Layout на Фрагмент</t>
+  </si>
+  <si>
+    <t>Main Act Main Fragment + MainViewModel</t>
+  </si>
+  <si>
+    <t>б.м. AndroidX но как-то неясно</t>
+  </si>
+  <si>
+    <t>NativeC++</t>
+  </si>
+  <si>
+    <t>Что-то делает с Эмулятором-2</t>
+  </si>
+  <si>
+    <t>Работает - вывел Hello C++</t>
+  </si>
+  <si>
+    <t>Material, ConstraintLyout appCompact</t>
+  </si>
+  <si>
+    <t>Main вызывает cpp</t>
+  </si>
+  <si>
+    <t>аще всего используется в качестве шаблона действия, чем в качестве шаблона модуля приложения.</t>
+  </si>
+  <si>
+    <t>Add_Template</t>
+  </si>
+  <si>
+    <t>добавляет прямо или в пакет</t>
+  </si>
+  <si>
+    <t>Add_Other</t>
+  </si>
+  <si>
+    <t>Добавляет но вызывать надо самому</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="45">
+  <fonts count="46">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11624,6 +11886,13 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -11736,7 +12005,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -11999,6 +12268,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -12676,6 +12949,1314 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910DE70C-3ACC-4B4B-BF23-64640DB3E5B8}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" style="51" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="51" customWidth="1"/>
+    <col min="3" max="3" width="23" style="51" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="51" customWidth="1"/>
+    <col min="5" max="5" width="17" style="51" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" style="51" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="51"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="51" t="s">
+        <v>3716</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="124" customFormat="1">
+      <c r="A2" s="124" t="s">
+        <v>3717</v>
+      </c>
+      <c r="B2" s="124" t="s">
+        <v>3746</v>
+      </c>
+      <c r="C2" s="124" t="s">
+        <v>3745</v>
+      </c>
+      <c r="D2" s="124" t="s">
+        <v>3744</v>
+      </c>
+      <c r="E2" s="124" t="s">
+        <v>3743</v>
+      </c>
+      <c r="F2" s="124" t="s">
+        <v>3729</v>
+      </c>
+      <c r="G2" s="124" t="s">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="51" t="s">
+        <v>3719</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>3720</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="51" t="s">
+        <v>3721</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>3722</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>3723</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>3725</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="51" t="s">
+        <v>3724</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>3727</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>3726</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>3738</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>3739</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>3731</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="51" t="s">
+        <v>3732</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>3733</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>3735</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>3737</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>3736</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="51" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>3742</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>3747</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>3748</v>
+      </c>
+      <c r="F7" s="51" t="s">
+        <v>3741</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="51" t="s">
+        <v>3749</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>3751</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>3752</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>3753</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>3750</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="51" t="s">
+        <v>3754</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>3755</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="F9" s="125" t="s">
+        <v>3756</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="51" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>3757</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>3761</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>3759</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>3758</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="51" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>3763</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>3764</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>3766</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>3767</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="51" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>3727</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>3770</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>3769</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>3739</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>3731</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="51" t="s">
+        <v>3771</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>3773</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>3775</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>3776</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>3772</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>3774</v>
+      </c>
+      <c r="I13" s="51" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="51" t="s">
+        <v>3777</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>3778</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>3779</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>3780</v>
+      </c>
+      <c r="G14" s="51" t="s">
+        <v>3781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="51" t="s">
+        <v>3782</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>3783</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>3784</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>3786</v>
+      </c>
+      <c r="F15" s="51" t="s">
+        <v>3785</v>
+      </c>
+      <c r="G15" s="51" t="s">
+        <v>3787</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="51" t="s">
+        <v>3788</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>3783</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>3718</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>3790</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>3789</v>
+      </c>
+      <c r="F16" s="51" t="s">
+        <v>3792</v>
+      </c>
+      <c r="G16" s="51" t="s">
+        <v>3791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="51" t="s">
+        <v>3793</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>3796</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>3794</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>3795</v>
+      </c>
+      <c r="G17" s="51" t="s">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="51" t="s">
+        <v>3799</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="51" t="s">
+        <v>3801</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>3802</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28110549-2348-49E2-B2A3-9BCD2CD81D05}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="86.42578125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>3187</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3188</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="75" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="117"/>
+      <c r="B2" s="118" t="s">
+        <v>3683</v>
+      </c>
+      <c r="C2" s="119" t="s">
+        <v>3190</v>
+      </c>
+      <c r="D2" s="74"/>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>3191</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>3192</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>3193</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>3194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A4" s="20">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>3195</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>3196</v>
+      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A5" s="20">
+        <v>3</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>3197</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>3198</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A6" s="20">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>3200</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>3201</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="20">
+        <v>5</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>3203</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>3204</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>3205</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="20">
+        <v>6</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>3207</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>3208</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="20">
+        <v>7</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>3210</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>3211</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>3212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A10" s="20">
+        <v>8</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>3213</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>3214</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>3215</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A11" s="20">
+        <v>9</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>3217</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>3218</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>3219</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="20">
+        <v>10</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>3221</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>3222</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>3223</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="29" customFormat="1" ht="30" customHeight="1">
+      <c r="A13" s="25">
+        <v>11</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>3225</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>3226</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>3227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" ht="21">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>3228</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.youtube.com/watch?v=DjDL5cjLYwE&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=2&amp;t=0s" xr:uid="{0B8D3BB2-4389-460D-ABAB-49DA68862A92}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://www.youtube.com/user/PlurrimiTube" xr:uid="{2ACEA3B7-42DE-4F25-8F57-041A1FDFB479}"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://www.youtube.com/watch?v=Ke_TKZaZGSI&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=3&amp;t=0s" xr:uid="{B2FC0E5D-3893-4D90-A8FF-9047ECC3F2F4}"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://www.youtube.com/watch?v=Omu-zBP_HCU&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=4&amp;t=0s" xr:uid="{1A2C2A24-4A67-4650-8ADD-A0B7A53C1B6C}"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://www.youtube.com/watch?v=Vq7zmySya7k&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=5&amp;t=0s" xr:uid="{4F1DB36C-9D02-45F6-9D81-4794346BE3B0}"/>
+    <hyperlink ref="C7" r:id="rId6" display="https://www.youtube.com/watch?v=r6MQ4VAHI_U&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=6&amp;t=0s" xr:uid="{3F13C209-5F22-4381-B37E-1A2D75B1F248}"/>
+    <hyperlink ref="C8" r:id="rId7" display="https://www.youtube.com/watch?v=hH4maqAdIQw&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=7&amp;t=0s" xr:uid="{EFE6C080-72E8-4797-82A3-3D9A68C0DECC}"/>
+    <hyperlink ref="C9" r:id="rId8" display="https://www.youtube.com/watch?v=Z_4OmuK_ZFM&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=8&amp;t=0s" xr:uid="{787CFEC9-42F6-4637-966D-ED63049DA970}"/>
+    <hyperlink ref="C10" r:id="rId9" display="https://www.youtube.com/watch?v=Zb4aABKDinY&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=9&amp;t=0s" xr:uid="{8741B8B8-AF71-48FD-B91B-2F2C9508FAB5}"/>
+    <hyperlink ref="C11" r:id="rId10" display="https://www.youtube.com/watch?v=eq5JhPYLFEE&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=10&amp;t=0s" xr:uid="{DE05D121-555B-4581-8AD8-87C29BA6C027}"/>
+    <hyperlink ref="C12" r:id="rId11" display="https://www.youtube.com/watch?v=V7wYHkigMJ4&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=11&amp;t=0s" xr:uid="{202337CB-0717-47E5-95A6-F186FA504001}"/>
+    <hyperlink ref="C13" r:id="rId12" display="https://www.youtube.com/watch?v=sHTbC3X4Dc4&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=12&amp;t=0s" xr:uid="{655F6A1B-6356-40A7-B526-973C7CB3A845}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B0B07-A8F9-4E90-B07A-F9B11F88923F}">
+  <dimension ref="A1:E89"/>
+  <sheetViews>
+    <sheetView topLeftCell="A79" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="16" t="s">
+        <v>3229</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3230</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>3231</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>3232</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>3234</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>3237</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>3188</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3189</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="26.25">
+      <c r="A11" s="31" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="26.25">
+      <c r="A12" s="31"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="17" t="s">
+        <v>3241</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>3242</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="17" t="s">
+        <v>3244</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>3245</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="17" t="s">
+        <v>3246</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>3247</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="17" t="s">
+        <v>3248</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>3249</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="17" t="s">
+        <v>3250</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>3251</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="17" t="s">
+        <v>3253</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>3254</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="17" t="s">
+        <v>3256</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>3257</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="17"/>
+      <c r="B20" s="32" t="s">
+        <v>3259</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="17" t="s">
+        <v>3261</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>3262</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="17"/>
+      <c r="B22" s="34" t="s">
+        <v>3264</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="35" t="s">
+        <v>3266</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>3267</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="17"/>
+      <c r="B24" s="32" t="s">
+        <v>3269</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="17" t="s">
+        <v>3271</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>3272</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45">
+      <c r="A26" s="36" t="s">
+        <v>3274</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>3275</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="35" t="s">
+        <v>3277</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>3278</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3279</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="35" t="s">
+        <v>3281</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>3282</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="17" t="s">
+        <v>3284</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>3285</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>3287</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3288</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="26.25">
+      <c r="A32" s="31" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="26.25">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+    </row>
+    <row r="34" spans="1:2" s="39" customFormat="1">
+      <c r="A34" s="38" t="s">
+        <v>3291</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>3292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="40" customFormat="1">
+      <c r="A35" s="40" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>2515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="40" customFormat="1">
+      <c r="A36" s="40" t="s">
+        <v>3293</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="40" customFormat="1">
+      <c r="A37" s="40" t="s">
+        <v>388</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>3295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="40" customFormat="1">
+      <c r="A38" s="40" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="40" customFormat="1">
+      <c r="A39" s="40" t="s">
+        <v>3296</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>3297</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="40" customFormat="1">
+      <c r="A40" s="40" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="40" customFormat="1">
+      <c r="A41" s="40" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="40" customFormat="1">
+      <c r="A42" s="40" t="s">
+        <v>3302</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>3303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="39" customFormat="1">
+      <c r="A44" s="38" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" s="40" customFormat="1">
+      <c r="A45" s="40" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>3307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="40" customFormat="1">
+      <c r="A46" s="40" t="s">
+        <v>3308</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="40" customFormat="1">
+      <c r="A47" s="40" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B47" s="40" t="s">
+        <v>3311</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="40" customFormat="1">
+      <c r="A48" s="40" t="s">
+        <v>3312</v>
+      </c>
+      <c r="B48" s="40" t="s">
+        <v>3313</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="40" customFormat="1">
+      <c r="A49" s="40" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>3315</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="39" customFormat="1">
+      <c r="A51" s="38" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="40" customFormat="1">
+      <c r="A52" s="40" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B52" s="40" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="41" customFormat="1">
+      <c r="A53" s="41" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="40" customFormat="1">
+      <c r="A54" s="40" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B54" s="40" t="s">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="41" customFormat="1">
+      <c r="A55" s="41" t="s">
+        <v>3324</v>
+      </c>
+      <c r="B55" s="41" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="40" customFormat="1">
+      <c r="A56" s="40" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" s="40" customFormat="1">
+      <c r="A59" s="40" t="s">
+        <v>3325</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="40" customFormat="1">
+      <c r="A60" s="40" t="s">
+        <v>3327</v>
+      </c>
+      <c r="B60" s="40" t="s">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="40" customFormat="1">
+      <c r="A61" s="40" t="s">
+        <v>3329</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="40" customFormat="1">
+      <c r="A62" s="40" t="s">
+        <v>3331</v>
+      </c>
+      <c r="B62" s="40" t="s">
+        <v>3332</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" s="40" customFormat="1">
+      <c r="A63" s="40" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B63" s="40" t="s">
+        <v>3334</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="41" customFormat="1">
+      <c r="A64" s="41" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B64" s="41" t="s">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="40" customFormat="1">
+      <c r="A65" s="40" t="s">
+        <v>3337</v>
+      </c>
+      <c r="B65" s="40" t="s">
+        <v>3338</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="40" customFormat="1">
+      <c r="A66" s="40" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B66" s="40" t="s">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="40" customFormat="1">
+      <c r="A67" s="40" t="s">
+        <v>3291</v>
+      </c>
+      <c r="B67" s="40" t="s">
+        <v>3292</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="40" customFormat="1">
+      <c r="A68" s="40" t="s">
+        <v>3341</v>
+      </c>
+      <c r="B68" s="40" t="s">
+        <v>3342</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="40" customFormat="1">
+      <c r="A69" s="40" t="s">
+        <v>3343</v>
+      </c>
+      <c r="B69" s="40" t="s">
+        <v>3344</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="41" customFormat="1">
+      <c r="A70" s="41" t="s">
+        <v>406</v>
+      </c>
+      <c r="B70" s="41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="40" customFormat="1">
+      <c r="A71" s="40" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B71" s="40" t="s">
+        <v>3346</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="40" customFormat="1">
+      <c r="A72" s="40" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B72" s="40" t="s">
+        <v>3348</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="9" t="s">
+        <v>3349</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>3351</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3352</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>3353</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3354</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>3355</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>3349</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>3359</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>3361</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>3363</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3364</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>3365</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>3367</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3368</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>3369</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>3371</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3372</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="http://github.com/pysaumont/fpinkotlin" xr:uid="{D6528AF9-EEEA-4F66-BBDF-8C1619F2E47F}"/>
+    <hyperlink ref="A4" r:id="rId2" display="http://github.com/pysaumont/fpinkotlin" xr:uid="{E30DD0F5-612D-4E8E-B90A-4E92713D9F37}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{AB1AC95F-CBD2-405A-BBAD-CE67C638A1A5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E165"/>
   <sheetViews>
@@ -13914,700 +15495,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1B0B07-A8F9-4E90-B07A-F9B11F88923F}">
-  <dimension ref="A1:E89"/>
-  <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
-        <v>3229</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3230</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>3231</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>3232</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>3233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
-        <v>3234</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
-        <v>3236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
-        <v>3237</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>3188</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3189</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3239</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="26.25">
-      <c r="A11" s="31" t="s">
-        <v>3240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="26.25">
-      <c r="A12" s="31"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="17" t="s">
-        <v>3241</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>3242</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3243</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="17" t="s">
-        <v>3244</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>3245</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="17" t="s">
-        <v>3246</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>3247</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3243</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="17" t="s">
-        <v>3248</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>3249</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="17" t="s">
-        <v>3250</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>3251</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3252</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="17" t="s">
-        <v>3253</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>3254</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3255</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="17" t="s">
-        <v>3256</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>3257</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3258</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="17"/>
-      <c r="B20" s="32" t="s">
-        <v>3259</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3260</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="17" t="s">
-        <v>3261</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>3262</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="17"/>
-      <c r="B22" s="34" t="s">
-        <v>3264</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="35" t="s">
-        <v>3266</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>3267</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3268</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="17"/>
-      <c r="B24" s="32" t="s">
-        <v>3269</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3270</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="17" t="s">
-        <v>3271</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>3272</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="45">
-      <c r="A26" s="36" t="s">
-        <v>3274</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>3275</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3276</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="35" t="s">
-        <v>3277</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>3278</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3279</v>
-      </c>
-      <c r="D27" t="s">
-        <v>3280</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="35" t="s">
-        <v>3281</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>3282</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3283</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="17" t="s">
-        <v>3284</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>3285</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3286</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>3287</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3288</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3289</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="26.25">
-      <c r="A32" s="31" t="s">
-        <v>3290</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>3290</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="26.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-    </row>
-    <row r="34" spans="1:2" s="39" customFormat="1">
-      <c r="A34" s="38" t="s">
-        <v>3291</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>3292</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="40" customFormat="1">
-      <c r="A35" s="40" t="s">
-        <v>2514</v>
-      </c>
-      <c r="B35" s="40" t="s">
-        <v>2515</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="40" customFormat="1">
-      <c r="A36" s="40" t="s">
-        <v>3293</v>
-      </c>
-      <c r="B36" s="40" t="s">
-        <v>3294</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="40" customFormat="1">
-      <c r="A37" s="40" t="s">
-        <v>388</v>
-      </c>
-      <c r="B37" s="40" t="s">
-        <v>3295</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" s="40" customFormat="1">
-      <c r="A38" s="40" t="s">
-        <v>2517</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>2518</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="40" customFormat="1">
-      <c r="A39" s="40" t="s">
-        <v>3296</v>
-      </c>
-      <c r="B39" s="40" t="s">
-        <v>3297</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" s="40" customFormat="1">
-      <c r="A40" s="40" t="s">
-        <v>3298</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>3299</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="40" customFormat="1">
-      <c r="A41" s="40" t="s">
-        <v>3300</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>3301</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="40" customFormat="1">
-      <c r="A42" s="40" t="s">
-        <v>3302</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>3303</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" s="39" customFormat="1">
-      <c r="A44" s="38" t="s">
-        <v>3304</v>
-      </c>
-      <c r="B44" s="38" t="s">
-        <v>3305</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" s="40" customFormat="1">
-      <c r="A45" s="40" t="s">
-        <v>3306</v>
-      </c>
-      <c r="B45" s="40" t="s">
-        <v>3307</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="40" customFormat="1">
-      <c r="A46" s="40" t="s">
-        <v>3308</v>
-      </c>
-      <c r="B46" s="40" t="s">
-        <v>3309</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" s="40" customFormat="1">
-      <c r="A47" s="40" t="s">
-        <v>3310</v>
-      </c>
-      <c r="B47" s="40" t="s">
-        <v>3311</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" s="40" customFormat="1">
-      <c r="A48" s="40" t="s">
-        <v>3312</v>
-      </c>
-      <c r="B48" s="40" t="s">
-        <v>3313</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" s="40" customFormat="1">
-      <c r="A49" s="40" t="s">
-        <v>3314</v>
-      </c>
-      <c r="B49" s="40" t="s">
-        <v>3315</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" s="39" customFormat="1">
-      <c r="A51" s="38" t="s">
-        <v>3316</v>
-      </c>
-      <c r="B51" s="38" t="s">
-        <v>3317</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" s="40" customFormat="1">
-      <c r="A52" s="40" t="s">
-        <v>3318</v>
-      </c>
-      <c r="B52" s="40" t="s">
-        <v>3319</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" s="41" customFormat="1">
-      <c r="A53" s="41" t="s">
-        <v>3320</v>
-      </c>
-      <c r="B53" s="41" t="s">
-        <v>3321</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" s="40" customFormat="1">
-      <c r="A54" s="40" t="s">
-        <v>3322</v>
-      </c>
-      <c r="B54" s="40" t="s">
-        <v>3323</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" s="41" customFormat="1">
-      <c r="A55" s="41" t="s">
-        <v>3324</v>
-      </c>
-      <c r="B55" s="41" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" s="40" customFormat="1">
-      <c r="A56" s="40" t="s">
-        <v>2112</v>
-      </c>
-      <c r="B56" s="40" t="s">
-        <v>2113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="9" t="s">
-        <v>393</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" s="40" customFormat="1">
-      <c r="A59" s="40" t="s">
-        <v>3325</v>
-      </c>
-      <c r="B59" s="40" t="s">
-        <v>3326</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="40" customFormat="1">
-      <c r="A60" s="40" t="s">
-        <v>3327</v>
-      </c>
-      <c r="B60" s="40" t="s">
-        <v>3328</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" s="40" customFormat="1">
-      <c r="A61" s="40" t="s">
-        <v>3329</v>
-      </c>
-      <c r="B61" s="40" t="s">
-        <v>3330</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" s="40" customFormat="1">
-      <c r="A62" s="40" t="s">
-        <v>3331</v>
-      </c>
-      <c r="B62" s="40" t="s">
-        <v>3332</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" s="40" customFormat="1">
-      <c r="A63" s="40" t="s">
-        <v>3333</v>
-      </c>
-      <c r="B63" s="40" t="s">
-        <v>3334</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" s="41" customFormat="1">
-      <c r="A64" s="41" t="s">
-        <v>3335</v>
-      </c>
-      <c r="B64" s="41" t="s">
-        <v>3336</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" s="40" customFormat="1">
-      <c r="A65" s="40" t="s">
-        <v>3337</v>
-      </c>
-      <c r="B65" s="40" t="s">
-        <v>3338</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" s="40" customFormat="1">
-      <c r="A66" s="40" t="s">
-        <v>3339</v>
-      </c>
-      <c r="B66" s="40" t="s">
-        <v>3340</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" s="40" customFormat="1">
-      <c r="A67" s="40" t="s">
-        <v>3291</v>
-      </c>
-      <c r="B67" s="40" t="s">
-        <v>3292</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" s="40" customFormat="1">
-      <c r="A68" s="40" t="s">
-        <v>3341</v>
-      </c>
-      <c r="B68" s="40" t="s">
-        <v>3342</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" s="40" customFormat="1">
-      <c r="A69" s="40" t="s">
-        <v>3343</v>
-      </c>
-      <c r="B69" s="40" t="s">
-        <v>3344</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" s="41" customFormat="1">
-      <c r="A70" s="41" t="s">
-        <v>406</v>
-      </c>
-      <c r="B70" s="41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" s="40" customFormat="1">
-      <c r="A71" s="40" t="s">
-        <v>3345</v>
-      </c>
-      <c r="B71" s="40" t="s">
-        <v>3346</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" s="40" customFormat="1">
-      <c r="A72" s="40" t="s">
-        <v>3347</v>
-      </c>
-      <c r="B72" s="40" t="s">
-        <v>3348</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="9" t="s">
-        <v>3349</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>3350</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
-        <v>3351</v>
-      </c>
-      <c r="B75" t="s">
-        <v>3352</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
-        <v>3353</v>
-      </c>
-      <c r="B76" t="s">
-        <v>3354</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>3355</v>
-      </c>
-      <c r="B77" t="s">
-        <v>3356</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
-        <v>3349</v>
-      </c>
-      <c r="B78" t="s">
-        <v>3350</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="9" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>3358</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
-        <v>3359</v>
-      </c>
-      <c r="B81" t="s">
-        <v>3360</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
-        <v>3361</v>
-      </c>
-      <c r="B82" t="s">
-        <v>3362</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
-        <v>3363</v>
-      </c>
-      <c r="B83" t="s">
-        <v>3364</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>3365</v>
-      </c>
-      <c r="B84" t="s">
-        <v>3366</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>3367</v>
-      </c>
-      <c r="B85" t="s">
-        <v>3368</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>3369</v>
-      </c>
-      <c r="B86" t="s">
-        <v>3370</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>3371</v>
-      </c>
-      <c r="B89" t="s">
-        <v>3372</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="http://github.com/pysaumont/fpinkotlin" xr:uid="{D6528AF9-EEEA-4F66-BBDF-8C1619F2E47F}"/>
-    <hyperlink ref="A4" r:id="rId2" display="http://github.com/pysaumont/fpinkotlin" xr:uid="{E30DD0F5-612D-4E8E-B90A-4E92713D9F37}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{AB1AC95F-CBD2-405A-BBAD-CE67C638A1A5}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0562A63-E2B7-435D-AC20-E5DDA4EF42AB}">
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A163" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
@@ -17067,7 +17959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C81E9D-2ACE-4DB9-8DAF-4BC792C707BE}">
   <dimension ref="A1:D145"/>
   <sheetViews>
@@ -18645,7 +19537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C248D1-DBC7-4A67-9CB0-AE385AFE6851}">
   <dimension ref="A1:D275"/>
   <sheetViews>
@@ -19297,7 +20189,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="30">
+    <row r="61" spans="1:3" ht="45">
       <c r="A61" s="13" t="s">
         <v>755</v>
       </c>
@@ -21089,7 +21981,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="30">
+    <row r="229" spans="1:3" ht="45">
       <c r="A229" s="13" t="s">
         <v>1237</v>
       </c>
@@ -21735,7 +22627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE17FB4-DB04-466D-BE7C-36E284E6ED8C}">
   <dimension ref="A1:C351"/>
   <sheetViews>
@@ -24583,7 +25475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79760926-713C-4A5C-BE5E-175B643CE1AC}">
   <dimension ref="A1:D303"/>
   <sheetViews>
@@ -28316,7 +29208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1466F8CC-20A7-4711-BFB3-9ED037CE23C6}">
   <dimension ref="A1:D341"/>
   <sheetViews>
@@ -30818,7 +31710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F60F87-DBD8-49E0-B507-948FDA248019}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -31183,239 +32075,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId39"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28110549-2348-49E2-B2A3-9BCD2CD81D05}">
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="86.42578125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" t="s">
-        <v>3187</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3188</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="75" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="117"/>
-      <c r="B2" s="118" t="s">
-        <v>3683</v>
-      </c>
-      <c r="C2" s="119" t="s">
-        <v>3190</v>
-      </c>
-      <c r="D2" s="74"/>
-    </row>
-    <row r="3" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="20">
-        <v>1</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>3191</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>3192</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>3193</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>3194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="20">
-        <v>2</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>3195</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>3196</v>
-      </c>
-      <c r="D4" s="23"/>
-    </row>
-    <row r="5" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A5" s="20">
-        <v>3</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>3197</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>3198</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="20">
-        <v>4</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>3200</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>3201</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>3202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="20">
-        <v>5</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>3203</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>3204</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>3205</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>3206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="20">
-        <v>6</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>3207</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>3208</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>3209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="20">
-        <v>7</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>3210</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>3211</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>3212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="20">
-        <v>8</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>3213</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>3214</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>3215</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>3216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="20">
-        <v>9</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>3217</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>3218</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>3219</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>3220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="16" customFormat="1" ht="30" customHeight="1">
-      <c r="A12" s="20">
-        <v>10</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>3221</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>3222</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>3223</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>3224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="29" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="25">
-        <v>11</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>3225</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>3226</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>3227</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="21">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19" t="s">
-        <v>3185</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>3228</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://www.youtube.com/watch?v=DjDL5cjLYwE&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=2&amp;t=0s" xr:uid="{0B8D3BB2-4389-460D-ABAB-49DA68862A92}"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://www.youtube.com/user/PlurrimiTube" xr:uid="{2ACEA3B7-42DE-4F25-8F57-041A1FDFB479}"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://www.youtube.com/watch?v=Ke_TKZaZGSI&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=3&amp;t=0s" xr:uid="{B2FC0E5D-3893-4D90-A8FF-9047ECC3F2F4}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://www.youtube.com/watch?v=Omu-zBP_HCU&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=4&amp;t=0s" xr:uid="{1A2C2A24-4A67-4650-8ADD-A0B7A53C1B6C}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://www.youtube.com/watch?v=Vq7zmySya7k&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=5&amp;t=0s" xr:uid="{4F1DB36C-9D02-45F6-9D81-4794346BE3B0}"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://www.youtube.com/watch?v=r6MQ4VAHI_U&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=6&amp;t=0s" xr:uid="{3F13C209-5F22-4381-B37E-1A2D75B1F248}"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://www.youtube.com/watch?v=hH4maqAdIQw&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=7&amp;t=0s" xr:uid="{EFE6C080-72E8-4797-82A3-3D9A68C0DECC}"/>
-    <hyperlink ref="C9" r:id="rId8" display="https://www.youtube.com/watch?v=Z_4OmuK_ZFM&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=8&amp;t=0s" xr:uid="{787CFEC9-42F6-4637-966D-ED63049DA970}"/>
-    <hyperlink ref="C10" r:id="rId9" display="https://www.youtube.com/watch?v=Zb4aABKDinY&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=9&amp;t=0s" xr:uid="{8741B8B8-AF71-48FD-B91B-2F2C9508FAB5}"/>
-    <hyperlink ref="C11" r:id="rId10" display="https://www.youtube.com/watch?v=eq5JhPYLFEE&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=10&amp;t=0s" xr:uid="{DE05D121-555B-4581-8AD8-87C29BA6C027}"/>
-    <hyperlink ref="C12" r:id="rId11" display="https://www.youtube.com/watch?v=V7wYHkigMJ4&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=11&amp;t=0s" xr:uid="{202337CB-0717-47E5-95A6-F186FA504001}"/>
-    <hyperlink ref="C13" r:id="rId12" display="https://www.youtube.com/watch?v=sHTbC3X4Dc4&amp;list=PL0lO_mIqDDFUP-pEWtX7mrnmoP4Hxxp6y&amp;index=12&amp;t=0s" xr:uid="{655F6A1B-6356-40A7-B526-973C7CB3A845}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId13"/>
-</worksheet>
 </file>
</xml_diff>